<commit_message>
mae mse and skydome
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X\Documents\INFOMGMT\WrldTmpl8-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB42FAC-E840-491C-8137-66F6E3F6C85F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54EE686C-C651-4D66-A8C2-B3C272EBF3F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5235" yWindow="3630" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:I47"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,7 +493,7 @@
     <col min="4" max="5" width="16" customWidth="1"/>
     <col min="6" max="7" width="16.7109375" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" customWidth="1"/>
-    <col min="9" max="9" width="26" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -730,28 +730,28 @@
         <v>15</v>
       </c>
       <c r="B10" s="6">
-        <v>1.3417E-2</v>
+        <v>4.4720000000000003E-3</v>
       </c>
       <c r="C10" s="6">
-        <v>1.4435999999999999E-2</v>
+        <v>4.8120000000000003E-3</v>
       </c>
       <c r="D10" s="6">
-        <v>2.4979999999999998E-3</v>
+        <v>8.7799999999999998E-4</v>
       </c>
       <c r="E10" s="6">
-        <v>3.7629999999999999E-3</v>
+        <v>1.307E-3</v>
       </c>
       <c r="F10" s="6">
-        <v>3.4738999999999999E-2</v>
+        <v>1.1591000000000001E-2</v>
       </c>
       <c r="G10" s="6">
-        <v>3.2932000000000003E-2</v>
+        <v>1.0984000000000001E-2</v>
       </c>
       <c r="H10" s="6">
-        <v>7.5584999999999999E-2</v>
+        <v>2.5194999999999999E-2</v>
       </c>
       <c r="I10" s="6">
-        <v>0.49812899999999999</v>
+        <v>0.166043</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -759,28 +759,28 @@
         <v>22</v>
       </c>
       <c r="B11" s="6">
-        <v>5.2694999999999999E-2</v>
+        <v>3.0145000000000002E-2</v>
       </c>
       <c r="C11" s="6">
-        <v>3.4543999999999998E-2</v>
+        <v>1.9896E-2</v>
       </c>
       <c r="D11" s="6">
-        <v>6.8279999999999999E-3</v>
+        <v>5.8520000000000004E-3</v>
       </c>
       <c r="E11" s="6">
-        <v>9.5510000000000005E-3</v>
+        <v>6.7120000000000001E-3</v>
       </c>
       <c r="F11" s="6">
-        <v>4.2757999999999997E-2</v>
+        <v>2.3532999999999998E-2</v>
       </c>
       <c r="G11" s="6">
-        <v>3.9965000000000001E-2</v>
+        <v>2.1996000000000002E-2</v>
       </c>
       <c r="H11" s="6">
-        <v>2.0954E-2</v>
+        <v>1.107E-2</v>
       </c>
       <c r="I11" s="6">
-        <v>2.7233E-2</v>
+        <v>1.4212000000000001E-2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -828,28 +828,28 @@
         <v>15</v>
       </c>
       <c r="B14" s="6">
-        <v>1.8870999999999999E-2</v>
+        <v>6.2899999999999996E-3</v>
       </c>
       <c r="C14" s="6">
-        <v>2.3959999999999999E-2</v>
+        <v>7.9869999999999993E-3</v>
       </c>
       <c r="D14" s="6">
-        <v>2.9007999999999999E-2</v>
+        <v>9.7160000000000007E-3</v>
       </c>
       <c r="E14" s="6">
-        <v>6.43E-3</v>
+        <v>2.1949999999999999E-3</v>
       </c>
       <c r="F14" s="6">
-        <v>2.5866E-2</v>
+        <v>8.6309999999999998E-3</v>
       </c>
       <c r="G14" s="6">
-        <v>0.33510000000000001</v>
+        <v>0.111707</v>
       </c>
       <c r="H14" s="6">
-        <v>2.5874000000000001E-2</v>
+        <v>8.6250000000000007E-3</v>
       </c>
       <c r="I14" s="6">
-        <v>3.8226000000000003E-2</v>
+        <v>1.2742E-2</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -857,28 +857,28 @@
         <v>22</v>
       </c>
       <c r="B15" s="6">
-        <v>5.4420000000000003E-2</v>
+        <v>3.1134999999999999E-2</v>
       </c>
       <c r="C15" s="6">
-        <v>3.5899E-2</v>
+        <v>2.0677000000000001E-2</v>
       </c>
       <c r="D15" s="6">
-        <v>6.9849999999999999E-3</v>
+        <v>5.9579999999999998E-3</v>
       </c>
       <c r="E15" s="6">
-        <v>9.8709999999999996E-3</v>
+        <v>6.8170000000000001E-3</v>
       </c>
       <c r="F15" s="6">
-        <v>4.3406E-2</v>
+        <v>2.3897999999999999E-2</v>
       </c>
       <c r="G15" s="6">
-        <v>4.1709999999999997E-2</v>
+        <v>2.2953999999999999E-2</v>
       </c>
       <c r="H15" s="6">
-        <v>2.0912E-2</v>
+        <v>1.1056E-2</v>
       </c>
       <c r="I15" s="6">
-        <v>2.6776000000000001E-2</v>
+        <v>1.3939999999999999E-2</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -915,28 +915,28 @@
         <v>15</v>
       </c>
       <c r="B18" s="6">
-        <v>2.6509000000000001E-2</v>
+        <v>8.8360000000000001E-3</v>
       </c>
       <c r="C18" s="6">
-        <v>3.8027999999999999E-2</v>
+        <v>1.2676E-2</v>
       </c>
       <c r="D18" s="6">
-        <v>7.5960000000000003E-3</v>
+        <v>2.5769999999999999E-3</v>
       </c>
       <c r="E18" s="6">
-        <v>4.3769999999999998E-3</v>
+        <v>1.511E-3</v>
       </c>
       <c r="F18" s="6">
-        <v>0.25229299999999999</v>
+        <v>8.4108000000000002E-2</v>
       </c>
       <c r="G18" s="6">
-        <v>0.114357</v>
+        <v>3.8126E-2</v>
       </c>
       <c r="H18" s="6">
-        <v>2.0378E-2</v>
+        <v>6.7930000000000004E-3</v>
       </c>
       <c r="I18" s="6">
-        <v>0.16076699999999999</v>
+        <v>5.3588999999999998E-2</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -944,28 +944,28 @@
         <v>22</v>
       </c>
       <c r="B19" s="6">
-        <v>5.6238000000000003E-2</v>
+        <v>3.2176999999999997E-2</v>
       </c>
       <c r="C19" s="6">
-        <v>3.7470000000000003E-2</v>
+        <v>2.1580999999999999E-2</v>
       </c>
       <c r="D19" s="6">
-        <v>7.0410000000000004E-3</v>
+        <v>5.9150000000000001E-3</v>
       </c>
       <c r="E19" s="6">
-        <v>9.9179999999999997E-3</v>
+        <v>6.8380000000000003E-3</v>
       </c>
       <c r="F19" s="6">
-        <v>4.6067999999999998E-2</v>
+        <v>2.5339E-2</v>
       </c>
       <c r="G19" s="6">
-        <v>4.308E-2</v>
+        <v>2.3701E-2</v>
       </c>
       <c r="H19" s="6">
-        <v>2.0871000000000001E-2</v>
+        <v>1.1036000000000001E-2</v>
       </c>
       <c r="I19" s="6">
-        <v>2.7484999999999999E-2</v>
+        <v>1.4349000000000001E-2</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1013,28 +1013,28 @@
         <v>15</v>
       </c>
       <c r="B22" s="6">
-        <v>7.5533000000000003E-2</v>
+        <v>2.5177999999999999E-2</v>
       </c>
       <c r="C22" s="6">
-        <v>4.7010999999999997E-2</v>
+        <v>1.567E-2</v>
       </c>
       <c r="D22" s="6">
-        <v>1.7321E-2</v>
+        <v>5.8190000000000004E-3</v>
       </c>
       <c r="E22" s="6">
-        <v>1.1557E-2</v>
+        <v>3.9050000000000001E-3</v>
       </c>
       <c r="F22" s="6">
-        <v>0.15603300000000001</v>
+        <v>5.2020999999999998E-2</v>
       </c>
       <c r="G22" s="6">
-        <v>1.2882199999999999</v>
+        <v>0.42941400000000002</v>
       </c>
       <c r="H22" s="6">
-        <v>4.0641999999999998E-2</v>
+        <v>1.3547E-2</v>
       </c>
       <c r="I22" s="6">
-        <v>3.3168999999999997E-2</v>
+        <v>1.1056E-2</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1042,28 +1042,28 @@
         <v>22</v>
       </c>
       <c r="B23" s="6">
-        <v>6.1780000000000002E-2</v>
+        <v>3.5355999999999999E-2</v>
       </c>
       <c r="C23" s="6">
-        <v>4.1013000000000001E-2</v>
+        <v>2.3622000000000001E-2</v>
       </c>
       <c r="D23" s="6">
-        <v>7.5339999999999999E-3</v>
+        <v>6.1040000000000001E-3</v>
       </c>
       <c r="E23" s="6">
-        <v>1.0418E-2</v>
+        <v>7.0219999999999996E-3</v>
       </c>
       <c r="F23" s="6">
-        <v>5.0203999999999999E-2</v>
+        <v>2.7660000000000001E-2</v>
       </c>
       <c r="G23" s="6">
-        <v>4.7389000000000001E-2</v>
+        <v>2.6010999999999999E-2</v>
       </c>
       <c r="H23" s="6">
-        <v>2.1559999999999999E-2</v>
+        <v>1.1394E-2</v>
       </c>
       <c r="I23" s="6">
-        <v>2.7902E-2</v>
+        <v>1.4496E-2</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1245,28 +1245,28 @@
         <v>15</v>
       </c>
       <c r="B31" s="6">
-        <v>1.4086E-2</v>
+        <v>4.6950000000000004E-3</v>
       </c>
       <c r="C31" s="6">
-        <v>1.2853E-2</v>
+        <v>4.2839999999999996E-3</v>
       </c>
       <c r="D31" s="6">
-        <v>1.474E-3</v>
+        <v>5.1800000000000001E-4</v>
       </c>
       <c r="E31" s="6">
-        <v>2.7880000000000001E-3</v>
+        <v>9.6599999999999995E-4</v>
       </c>
       <c r="F31" s="6">
-        <v>1.6608999999999999E-2</v>
+        <v>5.5430000000000002E-3</v>
       </c>
       <c r="G31" s="6">
-        <v>2.0296000000000002E-2</v>
+        <v>6.77E-3</v>
       </c>
       <c r="H31" s="6">
-        <v>3.5459999999999998E-2</v>
+        <v>1.1820000000000001E-2</v>
       </c>
       <c r="I31" s="6">
-        <v>4.2000000000000003E-2</v>
+        <v>1.4E-2</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1274,28 +1274,28 @@
         <v>22</v>
       </c>
       <c r="B32" s="6">
-        <v>6.0441000000000002E-2</v>
+        <v>3.4605999999999998E-2</v>
       </c>
       <c r="C32" s="6">
-        <v>3.7366000000000003E-2</v>
+        <v>2.1523E-2</v>
       </c>
       <c r="D32" s="6">
-        <v>1.2481000000000001E-2</v>
+        <v>7.4669999999999997E-3</v>
       </c>
       <c r="E32" s="6">
-        <v>1.5408E-2</v>
+        <v>8.8719999999999997E-3</v>
       </c>
       <c r="F32" s="6">
-        <v>5.2616000000000003E-2</v>
+        <v>2.8989000000000001E-2</v>
       </c>
       <c r="G32" s="6">
-        <v>4.6289999999999998E-2</v>
+        <v>2.5403999999999999E-2</v>
       </c>
       <c r="H32" s="6">
-        <v>8.1408999999999995E-2</v>
+        <v>3.9563000000000001E-2</v>
       </c>
       <c r="I32" s="6">
-        <v>8.8417999999999997E-2</v>
+        <v>4.2995999999999999E-2</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1589,25 +1589,25 @@
         <v>15</v>
       </c>
       <c r="B46" s="6">
-        <v>0.227798</v>
+        <v>7.5967000000000007E-2</v>
       </c>
       <c r="C46" s="6">
-        <v>0.15776599999999999</v>
+        <v>5.2597999999999999E-2</v>
       </c>
       <c r="D46" s="6">
-        <v>8.3611000000000005E-2</v>
+        <v>2.7945999999999999E-2</v>
       </c>
       <c r="E46" s="6">
-        <v>1.3939999999999999E-2</v>
+        <v>4.7080000000000004E-3</v>
       </c>
       <c r="F46" s="6">
-        <v>0.11293400000000001</v>
+        <v>3.7857000000000002E-2</v>
       </c>
       <c r="G46" s="6">
-        <v>0.157225</v>
+        <v>5.2748000000000003E-2</v>
       </c>
       <c r="H46" s="6">
-        <v>6.5039E-2</v>
+        <v>2.1683000000000001E-2</v>
       </c>
       <c r="I46" s="8" t="s">
         <v>20</v>
@@ -1618,25 +1618,25 @@
         <v>22</v>
       </c>
       <c r="B47" s="6">
-        <v>8.5380999999999999E-2</v>
+        <v>4.9123E-2</v>
       </c>
       <c r="C47" s="6">
-        <v>5.4737000000000001E-2</v>
+        <v>3.1572000000000003E-2</v>
       </c>
       <c r="D47" s="6">
-        <v>2.247E-2</v>
+        <v>1.3261E-2</v>
       </c>
       <c r="E47" s="6">
-        <v>1.7269E-2</v>
+        <v>1.0089000000000001E-2</v>
       </c>
       <c r="F47" s="6">
-        <v>7.3566999999999994E-2</v>
+        <v>4.1035000000000002E-2</v>
       </c>
       <c r="G47" s="6">
-        <v>7.2524000000000005E-2</v>
+        <v>4.0559999999999999E-2</v>
       </c>
       <c r="H47" s="6">
-        <v>5.4447000000000002E-2</v>
+        <v>2.7945999999999999E-2</v>
       </c>
       <c r="I47" s="8" t="s">
         <v>20</v>

</xml_diff>